<commit_message>
Ran alternative abstract measures
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_8_4.xlsx
+++ b/results/tables/final_tables_8_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EDF25E-FDA8-42DC-A261-0DD9735F858B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93665D3-A2BA-4BEE-9E17-0CFD69F9C9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="8" activeTab="10" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
@@ -1399,7 +1399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1562,6 +1562,8 @@
     <xf numFmtId="165" fontId="11" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1607,20 +1609,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2223,14 +2222,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="88" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
@@ -2332,14 +2331,14 @@
     </row>
     <row r="8" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="88" t="s">
         <v>277</v>
       </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
@@ -2468,20 +2467,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="86" t="s">
+      <c r="G2" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2796,11 +2795,11 @@
       <c r="B13" s="54">
         <v>62</v>
       </c>
-      <c r="G13" s="86" t="s">
+      <c r="G13" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="88"/>
       <c r="M13" s="81"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -2815,13 +2814,13 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="100"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="100"/>
+      <c r="B15" s="102"/>
+      <c r="C15" s="102"/>
+      <c r="D15" s="102"/>
+      <c r="E15" s="102"/>
       <c r="G15" s="18">
         <f t="shared" ref="G15:I17" si="10">+C18/$B18</f>
         <v>2.2692799840412765</v>
@@ -2965,11 +2964,11 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="G24" s="86" t="s">
+      <c r="G24" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="86"/>
-      <c r="I24" s="86"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
     </row>
     <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="G25" s="8" t="s">
@@ -2995,13 +2994,13 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="100" t="s">
+      <c r="A26" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="100"/>
-      <c r="C26" s="100"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="100"/>
+      <c r="B26" s="102"/>
+      <c r="C26" s="102"/>
+      <c r="D26" s="102"/>
+      <c r="E26" s="102"/>
       <c r="G26" s="18">
         <f t="shared" ref="G26:I28" si="11">+C29/$B29</f>
         <v>1.0840988998256753</v>
@@ -3178,20 +3177,20 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="100" t="s">
+      <c r="A37" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="100"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
-      <c r="E37" s="100"/>
+      <c r="B37" s="102"/>
+      <c r="C37" s="102"/>
+      <c r="D37" s="102"/>
+      <c r="E37" s="102"/>
     </row>
     <row r="38" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="86" t="s">
+      <c r="G38" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="86"/>
-      <c r="I38" s="86"/>
+      <c r="H38" s="88"/>
+      <c r="I38" s="88"/>
     </row>
     <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -3483,20 +3482,20 @@
       <c r="E49" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="100" t="s">
+      <c r="A51" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="100"/>
-      <c r="C51" s="100"/>
-      <c r="D51" s="100"/>
-      <c r="E51" s="100"/>
+      <c r="B51" s="102"/>
+      <c r="C51" s="102"/>
+      <c r="D51" s="102"/>
+      <c r="E51" s="102"/>
     </row>
     <row r="52" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G52" s="86" t="s">
+      <c r="G52" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="H52" s="86"/>
-      <c r="I52" s="86"/>
+      <c r="H52" s="88"/>
+      <c r="I52" s="88"/>
     </row>
     <row r="53" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
@@ -3821,7 +3820,7 @@
   <dimension ref="A2:S39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3832,7 +3831,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="87" t="s">
         <v>306</v>
       </c>
       <c r="B2" s="19"/>
@@ -3845,146 +3844,135 @@
       <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="103">
+      <c r="A3" s="86">
         <v>0</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" t="s">
         <v>235</v>
       </c>
-      <c r="C3" s="102" t="s">
+      <c r="C3" t="s">
         <v>236</v>
       </c>
-      <c r="D3" s="102" t="s">
+      <c r="D3" t="s">
         <v>237</v>
       </c>
-      <c r="E3" s="102" t="s">
+      <c r="E3" t="s">
         <v>238</v>
       </c>
-      <c r="F3" s="102" t="s">
+      <c r="F3" t="s">
         <v>239</v>
       </c>
-      <c r="G3" s="102" t="s">
+      <c r="G3" t="s">
         <v>244</v>
       </c>
-      <c r="H3" s="102" t="s">
+      <c r="H3" t="s">
         <v>240</v>
       </c>
-      <c r="I3" s="102" t="s">
+      <c r="I3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="103">
+      <c r="A4" s="86">
         <v>1</v>
       </c>
-      <c r="B4" s="102" t="s">
+      <c r="B4" t="s">
         <v>235</v>
       </c>
-      <c r="C4" s="102" t="s">
+      <c r="C4" t="s">
         <v>236</v>
       </c>
-      <c r="D4" s="102" t="s">
+      <c r="D4" t="s">
         <v>238</v>
       </c>
-      <c r="E4" s="102" t="s">
+      <c r="E4" t="s">
         <v>239</v>
       </c>
-      <c r="F4" s="102" t="s">
+      <c r="F4" t="s">
         <v>240</v>
       </c>
-      <c r="G4" s="102" t="s">
+      <c r="G4" t="s">
         <v>241</v>
       </c>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="103">
+      <c r="A5" s="86">
         <v>2</v>
       </c>
-      <c r="B5" s="102" t="s">
+      <c r="B5" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="102" t="s">
+      <c r="C5" t="s">
         <v>236</v>
       </c>
-      <c r="D5" s="102" t="s">
+      <c r="D5" t="s">
         <v>239</v>
       </c>
-      <c r="E5" s="102" t="s">
+      <c r="E5" t="s">
         <v>241</v>
       </c>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="103">
+      <c r="A6" s="86">
         <v>3</v>
       </c>
-      <c r="B6" s="102" t="s">
+      <c r="B6" t="s">
         <v>235</v>
       </c>
-      <c r="C6" s="102" t="s">
+      <c r="C6" t="s">
         <v>236</v>
       </c>
-      <c r="D6" s="102" t="s">
+      <c r="D6" t="s">
         <v>239</v>
       </c>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="105" t="s">
+      <c r="A9" s="104" t="s">
         <v>307</v>
       </c>
-      <c r="B9" s="105"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="105"/>
-      <c r="H9" s="105"/>
-      <c r="I9" s="105"/>
-      <c r="K9" s="106" t="s">
+      <c r="B9" s="104"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="104"/>
+      <c r="F9" s="104"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104"/>
+      <c r="K9" s="105" t="s">
         <v>308</v>
       </c>
-      <c r="L9" s="106"/>
-      <c r="M9" s="106"/>
-      <c r="N9" s="106"/>
-      <c r="O9" s="106"/>
-      <c r="P9" s="106"/>
-      <c r="Q9" s="106"/>
-      <c r="R9" s="106"/>
-      <c r="S9" s="106"/>
+      <c r="L9" s="105"/>
+      <c r="M9" s="105"/>
+      <c r="N9" s="105"/>
+      <c r="O9" s="105"/>
+      <c r="P9" s="105"/>
+      <c r="Q9" s="105"/>
+      <c r="R9" s="105"/>
+      <c r="S9" s="105"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="107" t="s">
+      <c r="A11" s="103" t="s">
         <v>309</v>
       </c>
-      <c r="B11" s="107"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="107"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="107"/>
-      <c r="K11" s="107" t="s">
+      <c r="B11" s="103"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="103"/>
+      <c r="F11" s="103"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="103"/>
+      <c r="K11" s="103" t="s">
         <v>309</v>
       </c>
-      <c r="L11" s="107"/>
-      <c r="M11" s="107"/>
-      <c r="N11" s="107"/>
-      <c r="O11" s="107"/>
-      <c r="P11" s="107"/>
-      <c r="Q11" s="107"/>
-      <c r="R11" s="107"/>
-      <c r="S11" s="107"/>
+      <c r="L11" s="103"/>
+      <c r="M11" s="103"/>
+      <c r="N11" s="103"/>
+      <c r="O11" s="103"/>
+      <c r="P11" s="103"/>
+      <c r="Q11" s="103"/>
+      <c r="R11" s="103"/>
+      <c r="S11" s="103"/>
     </row>
     <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4244,28 +4232,28 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="107" t="s">
+      <c r="A21" s="103" t="s">
         <v>310</v>
       </c>
-      <c r="B21" s="107"/>
-      <c r="C21" s="107"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="107"/>
-      <c r="H21" s="107"/>
-      <c r="I21" s="107"/>
-      <c r="K21" s="107" t="s">
+      <c r="B21" s="103"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="103"/>
+      <c r="E21" s="103"/>
+      <c r="F21" s="103"/>
+      <c r="G21" s="103"/>
+      <c r="H21" s="103"/>
+      <c r="I21" s="103"/>
+      <c r="K21" s="103" t="s">
         <v>310</v>
       </c>
-      <c r="L21" s="107"/>
-      <c r="M21" s="107"/>
-      <c r="N21" s="107"/>
-      <c r="O21" s="107"/>
-      <c r="P21" s="107"/>
-      <c r="Q21" s="107"/>
-      <c r="R21" s="107"/>
-      <c r="S21" s="107"/>
+      <c r="L21" s="103"/>
+      <c r="M21" s="103"/>
+      <c r="N21" s="103"/>
+      <c r="O21" s="103"/>
+      <c r="P21" s="103"/>
+      <c r="Q21" s="103"/>
+      <c r="R21" s="103"/>
+      <c r="S21" s="103"/>
     </row>
     <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4525,28 +4513,28 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="107" t="s">
+      <c r="A31" s="103" t="s">
         <v>311</v>
       </c>
-      <c r="B31" s="107"/>
-      <c r="C31" s="107"/>
-      <c r="D31" s="107"/>
-      <c r="E31" s="107"/>
-      <c r="F31" s="107"/>
-      <c r="G31" s="107"/>
-      <c r="H31" s="107"/>
-      <c r="I31" s="107"/>
-      <c r="K31" s="107" t="s">
+      <c r="B31" s="103"/>
+      <c r="C31" s="103"/>
+      <c r="D31" s="103"/>
+      <c r="E31" s="103"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="103"/>
+      <c r="H31" s="103"/>
+      <c r="I31" s="103"/>
+      <c r="K31" s="103" t="s">
         <v>311</v>
       </c>
-      <c r="L31" s="107"/>
-      <c r="M31" s="107"/>
-      <c r="N31" s="107"/>
-      <c r="O31" s="107"/>
-      <c r="P31" s="107"/>
-      <c r="Q31" s="107"/>
-      <c r="R31" s="107"/>
-      <c r="S31" s="107"/>
+      <c r="L31" s="103"/>
+      <c r="M31" s="103"/>
+      <c r="N31" s="103"/>
+      <c r="O31" s="103"/>
+      <c r="P31" s="103"/>
+      <c r="Q31" s="103"/>
+      <c r="R31" s="103"/>
+      <c r="S31" s="103"/>
     </row>
     <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="33" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4847,20 +4835,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="86" t="s">
+      <c r="G4" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -5181,10 +5169,10 @@
         <v>1.06E-5</v>
       </c>
       <c r="F10" s="28"/>
-      <c r="H10" s="101" t="s">
+      <c r="H10" s="106" t="s">
         <v>293</v>
       </c>
-      <c r="I10" s="101"/>
+      <c r="I10" s="106"/>
       <c r="L10" s="35"/>
     </row>
     <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5195,8 +5183,8 @@
       <c r="F11" s="28">
         <v>3.6207700000000002E-2</v>
       </c>
-      <c r="H11" s="101"/>
-      <c r="I11" s="101"/>
+      <c r="H11" s="106"/>
+      <c r="I11" s="106"/>
       <c r="L11" s="35"/>
       <c r="N11" s="35"/>
     </row>
@@ -5213,8 +5201,8 @@
       <c r="F12" s="28">
         <v>5.2985199999999999</v>
       </c>
-      <c r="H12" s="101"/>
-      <c r="I12" s="101"/>
+      <c r="H12" s="106"/>
+      <c r="I12" s="106"/>
       <c r="L12" s="35"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5230,8 +5218,8 @@
       <c r="F13" s="49">
         <v>30.137509999999999</v>
       </c>
-      <c r="H13" s="101"/>
-      <c r="I13" s="101"/>
+      <c r="H13" s="106"/>
+      <c r="I13" s="106"/>
       <c r="L13" s="35"/>
       <c r="N13" s="35"/>
     </row>
@@ -5399,8 +5387,8 @@
       <c r="E33" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H33" s="90"/>
-      <c r="I33" s="90"/>
+      <c r="H33" s="92"/>
+      <c r="I33" s="92"/>
       <c r="L33" s="35"/>
     </row>
     <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5408,10 +5396,10 @@
         <v>290</v>
       </c>
       <c r="O34" s="79"/>
-      <c r="P34" s="90" t="s">
+      <c r="P34" s="92" t="s">
         <v>280</v>
       </c>
-      <c r="Q34" s="90"/>
+      <c r="Q34" s="92"/>
     </row>
     <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="10" t="s">
@@ -5541,10 +5529,10 @@
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C40" s="9"/>
       <c r="F40" s="28"/>
-      <c r="H40" s="101" t="s">
+      <c r="H40" s="106" t="s">
         <v>293</v>
       </c>
-      <c r="I40" s="101"/>
+      <c r="I40" s="106"/>
       <c r="K40" t="s">
         <v>288</v>
       </c>
@@ -5562,8 +5550,8 @@
       <c r="F41" s="28">
         <v>1.365048</v>
       </c>
-      <c r="H41" s="101"/>
-      <c r="I41" s="101"/>
+      <c r="H41" s="106"/>
+      <c r="I41" s="106"/>
       <c r="K41" t="s">
         <v>289</v>
       </c>
@@ -5576,8 +5564,8 @@
       <c r="F42" s="28">
         <v>-0.3439432</v>
       </c>
-      <c r="H42" s="101"/>
-      <c r="I42" s="101"/>
+      <c r="H42" s="106"/>
+      <c r="I42" s="106"/>
     </row>
     <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="35">
@@ -5592,8 +5580,8 @@
       <c r="F43" s="49">
         <v>13.51919</v>
       </c>
-      <c r="H43" s="101"/>
-      <c r="I43" s="101"/>
+      <c r="H43" s="106"/>
+      <c r="I43" s="106"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B44" s="35">
@@ -7012,12 +7000,12 @@
       <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7581,66 +7569,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="89" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
       <c r="G1" s="54"/>
-      <c r="H1" s="87" t="s">
+      <c r="H1" s="89" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="N1" s="87" t="s">
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="N1" s="89" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="T1" s="87" t="s">
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="T1" s="89" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="89"/>
+      <c r="W1" s="89"/>
+      <c r="X1" s="89"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="90" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="88" t="s">
+      <c r="H2" s="90" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="N2" s="88" t="s">
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="N2" s="90" t="s">
         <v>214</v>
       </c>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
-      <c r="T2" s="88" t="s">
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90"/>
+      <c r="T2" s="90" t="s">
         <v>214</v>
       </c>
-      <c r="U2" s="89"/>
-      <c r="V2" s="89"/>
-      <c r="W2" s="89"/>
-      <c r="X2" s="89"/>
+      <c r="U2" s="91"/>
+      <c r="V2" s="91"/>
+      <c r="W2" s="91"/>
+      <c r="X2" s="91"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -8675,10 +8663,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="92" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="90"/>
+      <c r="C2" s="92"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -9213,13 +9201,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -9333,12 +9321,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="92" t="s">
+      <c r="A10" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="92"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="92"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -9637,12 +9625,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="92" t="s">
+      <c r="A37" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="92"/>
-      <c r="C37" s="92"/>
-      <c r="D37" s="92"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -9976,13 +9964,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="95" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -10220,13 +10208,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="94" t="s">
+      <c r="A21" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="94"/>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="94"/>
+      <c r="B21" s="96"/>
+      <c r="C21" s="96"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="96"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="50"/>
@@ -10254,13 +10242,13 @@
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="93" t="s">
+      <c r="A25" s="95" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="93"/>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="93"/>
+      <c r="B25" s="95"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="95"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
@@ -10522,13 +10510,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="94" t="s">
+      <c r="A43" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="94"/>
-      <c r="C43" s="94"/>
-      <c r="D43" s="94"/>
-      <c r="E43" s="94"/>
+      <c r="B43" s="96"/>
+      <c r="C43" s="96"/>
+      <c r="D43" s="96"/>
+      <c r="E43" s="96"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -10896,36 +10884,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="95"/>
-      <c r="R3" s="95"/>
-      <c r="S3" s="95"/>
-      <c r="T3" s="95"/>
-      <c r="U3" s="95"/>
-      <c r="V3" s="95"/>
-      <c r="W3" s="95"/>
-      <c r="X3" s="95"/>
-      <c r="Y3" s="95"/>
-      <c r="Z3" s="95"/>
-      <c r="AA3" s="95"/>
-      <c r="AB3" s="95"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="97"/>
+      <c r="T3" s="97"/>
+      <c r="U3" s="97"/>
+      <c r="V3" s="97"/>
+      <c r="W3" s="97"/>
+      <c r="X3" s="97"/>
+      <c r="Y3" s="97"/>
+      <c r="Z3" s="97"/>
+      <c r="AA3" s="97"/>
+      <c r="AB3" s="97"/>
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -11444,35 +11432,35 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="99" t="s">
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="96" t="s">
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="97" t="s">
+      <c r="L4" s="98"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="97"/>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="97"/>
-      <c r="T4" s="97"/>
-      <c r="U4" s="97"/>
-      <c r="V4" s="97"/>
+      <c r="P4" s="99"/>
+      <c r="Q4" s="99"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="99"/>
+      <c r="U4" s="99"/>
+      <c r="V4" s="99"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">

</xml_diff>